<commit_message>
Se resuelve ingreso a Comprobantes en Línea, se agrega cierre de sesión
</commit_message>
<xml_diff>
--- a/Datos.xlsx
+++ b/Datos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Supervisor\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Proyectos\AFIP-Descarga-FC-Extraccion-Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B091C762-074E-4C9D-AD2B-6AC0E558E78A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB418F4A-CDBA-420D-A97D-09EACBDB91D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,16 +36,16 @@
     <t>Nombre completo</t>
   </si>
   <si>
-    <t>Contraseña</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RAZON SOCIAL </t>
-  </si>
-  <si>
     <t>desde</t>
   </si>
   <si>
     <t>hasta</t>
+  </si>
+  <si>
+    <t>fakestreet123</t>
+  </si>
+  <si>
+    <t>COSME FULANITO</t>
   </si>
 </sst>
 </file>
@@ -392,18 +392,18 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
-    <col min="4" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -414,21 +414,21 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>20000000001</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>20111111112</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D2" s="2">
         <v>44927</v>

</xml_diff>